<commit_message>
PDF Print Service Articulation Test Refactoring
</commit_message>
<xml_diff>
--- a/Doc/articulation_test_eng.xlsx
+++ b/Doc/articulation_test_eng.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SpeechPathology\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SpeechPathology\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{24A01985-05CB-4437-9591-7A96EC8E3A58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A636238-5092-4191-862D-F86AD74FAAC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{DDB625DF-4F01-4CCA-920B-D59ABAD0D606}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="117">
   <si>
     <t>Sounds</t>
   </si>
@@ -364,7 +364,22 @@
     <t>Image</t>
   </si>
   <si>
-    <t>lemon.png</t>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Medial</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Blended</t>
+  </si>
+  <si>
+    <t>lemon.jpg</t>
+  </si>
+  <si>
+    <t>book.jpg</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ED3D1D-554F-4288-BEE9-9630FEF3B2C4}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E81"/>
     </sheetView>
   </sheetViews>
@@ -1257,14 +1272,14 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('m','mole','INITIAL','lemon.png');</v>
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','mole','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1275,14 +1290,14 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('n','nut','INITIAL','lemon.png');</v>
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','nut','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1293,14 +1308,14 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('h','hen','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('h','hen','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1311,14 +1326,14 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('p','pig','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','pig','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1329,14 +1344,14 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('b','boot','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','boot','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1347,14 +1362,14 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('t','train','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','train','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1365,14 +1380,14 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('k','cat','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','cat','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1383,14 +1398,14 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('w','wolf','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','wolf','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1401,14 +1416,14 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('d','dog','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','dog','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1419,14 +1434,14 @@
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('g','gate','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','gate','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1437,14 +1452,14 @@
         <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('f','finger','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','finger','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1455,14 +1470,14 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('l','log','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','log','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1473,14 +1488,14 @@
         <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('s','sun','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','sun','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1491,14 +1506,14 @@
         <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('v','van','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('v','van','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1509,14 +1524,14 @@
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('y','yak','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','yak','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1527,14 +1542,14 @@
         <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ch','chips','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','chips','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1545,14 +1560,14 @@
         <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('r','rat','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','rat','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1563,14 +1578,14 @@
         <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('j','jam','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','jam','Initial','lemon.jpg');</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1581,14 +1596,14 @@
         <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D20" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('sh','shower','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('sh','shower','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1599,14 +1614,14 @@
         <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('th','thistle','INITIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('th','thistle','Initial','book.jpg');</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1617,14 +1632,14 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('m','lemon','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','lemon','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1635,14 +1650,14 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('n','dinner','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','dinner','Medial','book.jpg');</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1653,14 +1668,14 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('h','foghorn','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('h','foghorn','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1671,14 +1686,14 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('p','slipper','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','slipper','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1689,14 +1704,14 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('b','robot','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','robot','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1707,14 +1722,14 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('t','water','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','water','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1725,14 +1740,14 @@
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('k','rocket','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','rocket','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1743,14 +1758,14 @@
         <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('w','tower','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','tower','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1761,14 +1776,14 @@
         <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('d','puddle','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','puddle','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1779,14 +1794,14 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('g','tiger','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','tiger','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1797,14 +1812,14 @@
         <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('f','wafer','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','wafer','Medial','book.jpg');</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1815,14 +1830,14 @@
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ng','finger','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ng','finger','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1833,14 +1848,14 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('l','tulip','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','tulip','Medial','book.jpg');</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1851,14 +1866,14 @@
         <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('s','buses','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','buses','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1869,14 +1884,14 @@
         <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('v','waving','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('v','waving','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1887,14 +1902,14 @@
         <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('y','crayon','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','crayon','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1905,14 +1920,14 @@
         <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ch','archer','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','archer','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1923,14 +1938,14 @@
         <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('r','barrel','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','barrel','Medial','book.jpg');</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1941,14 +1956,14 @@
         <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('j','badger','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','badger','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1959,14 +1974,14 @@
         <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('sh','bishop','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('sh','bishop','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1977,14 +1992,14 @@
         <v>102</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('th','father','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('th','father','Medial','book.jpg');</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1995,14 +2010,14 @@
         <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('zh','measure','MEDIAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('zh','measure','Medial','lemon.jpg');</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2013,14 +2028,14 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('m','thumb','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','thumb','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2031,14 +2046,14 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('n','pin','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','pin','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2049,14 +2064,14 @@
         <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('p','map','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','map','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -2067,14 +2082,14 @@
         <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('b','cub','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','cub','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -2085,14 +2100,14 @@
         <v>33</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('t','hat','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','hat','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2103,14 +2118,14 @@
         <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('k','sock','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','sock','Final','book.jpg');</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -2121,14 +2136,14 @@
         <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D50" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('w','cow','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','cow','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -2139,14 +2154,14 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('d','head','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','head','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2157,14 +2172,14 @@
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D52" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('g','bag','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','bag','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2175,14 +2190,14 @@
         <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('f','laugh','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','laugh','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2193,14 +2208,14 @@
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D54" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ng','wing','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ng','wing','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2211,14 +2226,14 @@
         <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('l','hill','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','hill','Final','book.jpg');</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2229,14 +2244,14 @@
         <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D56" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('s','moose','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','moose','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2247,14 +2262,14 @@
         <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D57" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('v','sieve','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('v','sieve','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2265,14 +2280,14 @@
         <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('y','toy','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','toy','Final','book.jpg');</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2283,14 +2298,14 @@
         <v>84</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ch','witch','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','witch','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2301,14 +2316,14 @@
         <v>89</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D60" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('r','car','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','car','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2319,14 +2334,14 @@
         <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D61" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('j','midge','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','midge','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2337,14 +2352,14 @@
         <v>99</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('sh','fish','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('sh','fish','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2355,14 +2370,14 @@
         <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('th','path','FINAL','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('th','path','Final','lemon.jpg');</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2373,14 +2388,14 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('m','mummy','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','mummy','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2391,14 +2406,14 @@
         <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('n','cannon','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','cannon','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2409,14 +2424,14 @@
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('h','hardhat','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('h','hardhat','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2427,14 +2442,14 @@
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E81" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('p','pepper','BLENDED','lemon.png');</v>
+        <f t="shared" ref="E67:E81" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','pepper','Blended','book.jpg');</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2445,14 +2460,14 @@
         <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('b','baby','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','baby','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2463,14 +2478,14 @@
         <v>34</v>
       </c>
       <c r="C69" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D69" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('t','tent','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','tent','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2481,14 +2496,14 @@
         <v>39</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('k','cockerel','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','cockerel','Blended','book.jpg');</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2499,14 +2514,14 @@
         <v>44</v>
       </c>
       <c r="C71" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D71" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('w','window','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','window','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -2517,14 +2532,14 @@
         <v>49</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D72" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('d','daddy','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','daddy','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2535,14 +2550,14 @@
         <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('g','goggles','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','goggles','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -2553,14 +2568,14 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D74" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('f','fifteen','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','fifteen','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -2571,14 +2586,14 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D75" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ng','swinging','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ng','swinging','Blended','book.jpg');</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -2589,14 +2604,14 @@
         <v>67</v>
       </c>
       <c r="C76" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D76" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('l','lollipop','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','lollipop','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2607,14 +2622,14 @@
         <v>70</v>
       </c>
       <c r="C77" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D77" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('s','buses','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','buses','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2625,14 +2640,14 @@
         <v>80</v>
       </c>
       <c r="C78" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D78" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('y','yoyo','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','yoyo','Blended','book.jpg');</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2643,14 +2658,14 @@
         <v>85</v>
       </c>
       <c r="C79" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D79" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('ch','church','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','church','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2661,14 +2676,14 @@
         <v>90</v>
       </c>
       <c r="C80" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D80" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('r','robber','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','robber','Blended','lemon.jpg');</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2679,14 +2694,14 @@
         <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="D81" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[Position],[Image])  VALUES ('j','george','BLENDED','lemon.png');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','george','Blended','book.jpg');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TR Language Images New SVG logo for Erasmus+ Added LanguageCode field in ArticulationTest model
</commit_message>
<xml_diff>
--- a/Doc/articulation_test_eng.xlsx
+++ b/Doc/articulation_test_eng.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SpeechPathology\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A636238-5092-4191-862D-F86AD74FAAC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5246E9-BA88-48B1-A587-CF551B7F4CA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{DDB625DF-4F01-4CCA-920B-D59ABAD0D606}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3" xr2:uid="{DDB625DF-4F01-4CCA-920B-D59ABAD0D606}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ENG_DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="ENG_SQL" sheetId="2" r:id="rId2"/>
+    <sheet name="TR_DATA" sheetId="3" r:id="rId3"/>
+    <sheet name="TR_SQL" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ENG_SQL!$A$1:$E$81</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="262">
   <si>
     <t>Sounds</t>
   </si>
@@ -380,13 +383,448 @@
   </si>
   <si>
     <t>book.jpg</t>
+  </si>
+  <si>
+    <t>LETTER</t>
+  </si>
+  <si>
+    <t>bardak</t>
+  </si>
+  <si>
+    <t>kibrit</t>
+  </si>
+  <si>
+    <t>bebek</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>cep</t>
+  </si>
+  <si>
+    <t>gece</t>
+  </si>
+  <si>
+    <t>cüce</t>
+  </si>
+  <si>
+    <t>ç</t>
+  </si>
+  <si>
+    <t>çocuk</t>
+  </si>
+  <si>
+    <t>uçak</t>
+  </si>
+  <si>
+    <t>havuç</t>
+  </si>
+  <si>
+    <t>çiçek</t>
+  </si>
+  <si>
+    <t>diş</t>
+  </si>
+  <si>
+    <t>ördek</t>
+  </si>
+  <si>
+    <t>dede</t>
+  </si>
+  <si>
+    <t>fırça</t>
+  </si>
+  <si>
+    <t>köfte</t>
+  </si>
+  <si>
+    <t>muz</t>
+  </si>
+  <si>
+    <t>fotograf</t>
+  </si>
+  <si>
+    <t>gözlük</t>
+  </si>
+  <si>
+    <t>sünger</t>
+  </si>
+  <si>
+    <t>puding</t>
+  </si>
+  <si>
+    <t>gaga</t>
+  </si>
+  <si>
+    <t>hamur</t>
+  </si>
+  <si>
+    <t>anahtar</t>
+  </si>
+  <si>
+    <t>siyah</t>
+  </si>
+  <si>
+    <t>kedi</t>
+  </si>
+  <si>
+    <t>şeker</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>bakkal</t>
+  </si>
+  <si>
+    <t>lamba</t>
+  </si>
+  <si>
+    <t>telefon</t>
+  </si>
+  <si>
+    <t>fil</t>
+  </si>
+  <si>
+    <t>lale</t>
+  </si>
+  <si>
+    <t>makas</t>
+  </si>
+  <si>
+    <t>limon</t>
+  </si>
+  <si>
+    <t>kalem</t>
+  </si>
+  <si>
+    <t>mum</t>
+  </si>
+  <si>
+    <t>nar</t>
+  </si>
+  <si>
+    <t>salıncak</t>
+  </si>
+  <si>
+    <t>burun</t>
+  </si>
+  <si>
+    <t>ananas</t>
+  </si>
+  <si>
+    <t>portakal</t>
+  </si>
+  <si>
+    <t>süpürge</t>
+  </si>
+  <si>
+    <t>kalp</t>
+  </si>
+  <si>
+    <t>paspas</t>
+  </si>
+  <si>
+    <t>resim</t>
+  </si>
+  <si>
+    <t>mantar</t>
+  </si>
+  <si>
+    <t>rüzgar</t>
+  </si>
+  <si>
+    <t>sabun</t>
+  </si>
+  <si>
+    <t>taksi</t>
+  </si>
+  <si>
+    <t>dans</t>
+  </si>
+  <si>
+    <t>seksen</t>
+  </si>
+  <si>
+    <t>ş</t>
+  </si>
+  <si>
+    <t>şapka</t>
+  </si>
+  <si>
+    <t>kaşık</t>
+  </si>
+  <si>
+    <t>güneş</t>
+  </si>
+  <si>
+    <t>şişman</t>
+  </si>
+  <si>
+    <t>tabak</t>
+  </si>
+  <si>
+    <t>yastık</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>vişne</t>
+  </si>
+  <si>
+    <t>tavşan</t>
+  </si>
+  <si>
+    <t>ev</t>
+  </si>
+  <si>
+    <t>civciv</t>
+  </si>
+  <si>
+    <t>yatak</t>
+  </si>
+  <si>
+    <t>çay</t>
+  </si>
+  <si>
+    <t>yay</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>zil</t>
+  </si>
+  <si>
+    <t>üzüm</t>
+  </si>
+  <si>
+    <t>karpuz</t>
+  </si>
+  <si>
+    <t>gazoz</t>
+  </si>
+  <si>
+    <t>bardak.png</t>
+  </si>
+  <si>
+    <t>cep.png</t>
+  </si>
+  <si>
+    <t>çocuk.png</t>
+  </si>
+  <si>
+    <t>diş.png</t>
+  </si>
+  <si>
+    <t>fırça.png</t>
+  </si>
+  <si>
+    <t>gözlük.png</t>
+  </si>
+  <si>
+    <t>kedi.png</t>
+  </si>
+  <si>
+    <t>lamba.png</t>
+  </si>
+  <si>
+    <t>makas.png</t>
+  </si>
+  <si>
+    <t>portakal.png</t>
+  </si>
+  <si>
+    <t>resim.png</t>
+  </si>
+  <si>
+    <t>sabun.png</t>
+  </si>
+  <si>
+    <t>şapka.png</t>
+  </si>
+  <si>
+    <t>tabak.png</t>
+  </si>
+  <si>
+    <t>vişne.png</t>
+  </si>
+  <si>
+    <t>yatak.png</t>
+  </si>
+  <si>
+    <t>zil.png</t>
+  </si>
+  <si>
+    <t>kibrit.png</t>
+  </si>
+  <si>
+    <t>gece.png</t>
+  </si>
+  <si>
+    <t>uçak.png</t>
+  </si>
+  <si>
+    <t>ördek.png</t>
+  </si>
+  <si>
+    <t>sünger.png</t>
+  </si>
+  <si>
+    <t>anahtar.png</t>
+  </si>
+  <si>
+    <t>şeker.png</t>
+  </si>
+  <si>
+    <t>telefon.png</t>
+  </si>
+  <si>
+    <t>limon.png</t>
+  </si>
+  <si>
+    <t>salıncak.png</t>
+  </si>
+  <si>
+    <t>süpürge.png</t>
+  </si>
+  <si>
+    <t>kaşık.png</t>
+  </si>
+  <si>
+    <t>yastık.png</t>
+  </si>
+  <si>
+    <t>tavşan.png</t>
+  </si>
+  <si>
+    <t>siyah.png</t>
+  </si>
+  <si>
+    <t>üzüm.png</t>
+  </si>
+  <si>
+    <t>havuç.png</t>
+  </si>
+  <si>
+    <t>puding.png</t>
+  </si>
+  <si>
+    <t>park.png</t>
+  </si>
+  <si>
+    <t>fil.png</t>
+  </si>
+  <si>
+    <t>kalem.png</t>
+  </si>
+  <si>
+    <t>burun.png</t>
+  </si>
+  <si>
+    <t>kalp.png</t>
+  </si>
+  <si>
+    <t>mantar.png</t>
+  </si>
+  <si>
+    <t>dans.png</t>
+  </si>
+  <si>
+    <t>güneş.png</t>
+  </si>
+  <si>
+    <t>at.png</t>
+  </si>
+  <si>
+    <t>ev.png</t>
+  </si>
+  <si>
+    <t>bebek.png</t>
+  </si>
+  <si>
+    <t>çiçek.png</t>
+  </si>
+  <si>
+    <t>dede.png</t>
+  </si>
+  <si>
+    <t>gaga.png</t>
+  </si>
+  <si>
+    <t>mum.png</t>
+  </si>
+  <si>
+    <t>paspas.png</t>
+  </si>
+  <si>
+    <t>rüzgar.png</t>
+  </si>
+  <si>
+    <t>yay.png</t>
+  </si>
+  <si>
+    <t>fotograf.jpg</t>
+  </si>
+  <si>
+    <t>taksi.jpg</t>
+  </si>
+  <si>
+    <t>ananas.jpg</t>
+  </si>
+  <si>
+    <t>bakkal.jpg</t>
+  </si>
+  <si>
+    <t>civciv.jpg</t>
+  </si>
+  <si>
+    <t>hamur.jpg</t>
+  </si>
+  <si>
+    <t>karpuz.jpg</t>
+  </si>
+  <si>
+    <t>lale.jpg</t>
+  </si>
+  <si>
+    <t>muz.jpg</t>
+  </si>
+  <si>
+    <t>nar.jpg</t>
+  </si>
+  <si>
+    <t>seksen.jpg</t>
+  </si>
+  <si>
+    <t>tablet.jpg</t>
+  </si>
+  <si>
+    <t>cüce.jpg</t>
+  </si>
+  <si>
+    <t>köfte.jpg</t>
+  </si>
+  <si>
+    <t>çay.jpg</t>
+  </si>
+  <si>
+    <t>şişman.jpg</t>
+  </si>
+  <si>
+    <t>gazoz.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,8 +860,25 @@
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,8 +891,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -445,11 +906,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -462,9 +939,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1236,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ED3D1D-554F-4288-BEE9-9630FEF3B2C4}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2707,4 +3188,1701 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DF3CA4-88C8-4DD8-82AB-1500BC354F4E}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7C40D4-1A8C-49B8-AC4C-BD9FDA66D6CE}">
+  <dimension ref="A1:E73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="98.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"', 'TR');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','bardak','Initial','bardak.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"', 'TR');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('c','cep','Initial','cep.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','çocuk','Initial','çocuk.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','diş','Initial','diş.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fırça','Initial','fırça.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gözlük','Initial','gözlük.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hamur','Initial','hamur.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','kedi','Initial','kedi.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lamba','Initial','lamba.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','makas','Initial','makas.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','nar','Initial','nar.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','portakal','Initial','portakal.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','resim','Initial','resim.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','sabun','Initial','sabun.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','şapka','Initial','şapka.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tabak','Initial','tabak.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','vişne','Initial','vişne.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yatak','Initial','yatak.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','zil','Initial','zil.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','kibrit','Medial','kibrit.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('c','gece','Medial','gece.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','uçak','Medial','uçak.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','ördek','Medial','ördek.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>258</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','köfte','Medial','köfte.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','sünger','Medial','sünger.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','anahtar','Medial','anahtar.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','şeker','Medial','şeker.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','telefon','Medial','telefon.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" t="s">
+        <v>217</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','limon','Medial','limon.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" t="s">
+        <v>218</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','salıncak','Medial','salıncak.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" t="s">
+        <v>219</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','süpürge','Medial','süpürge.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','fırça','Medial','fırça.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','taksi','Medial','taksi.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="s">
+        <v>220</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','kaşık','Medial','kaşık.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
+        <v>221</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','yastık','Medial','yastık.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','tavşan','Medial','tavşan.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','siyah','Medial','siyah.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" t="s">
+        <v>224</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','üzüm','Medial','üzüm.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','havuç','Final','havuç.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" t="s">
+        <v>253</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','muz','Final','muz.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" t="s">
+        <v>226</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','puding','Final','puding.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" t="s">
+        <v>223</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','siyah','Final','siyah.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" t="s">
+        <v>227</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','park','Final','park.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" t="s">
+        <v>228</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','fil','Final','fil.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','kalem','Final','kalem.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" t="s">
+        <v>230</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','burun','Final','burun.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','kalp','Final','kalp.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" t="s">
+        <v>232</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','mantar','Final','mantar.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" t="s">
+        <v>233</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','dans','Final','dans.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" t="s">
+        <v>234</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','güneş','Final','güneş.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" t="s">
+        <v>235</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','at','Final','at.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" t="s">
+        <v>236</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','ev','Final','ev.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" t="s">
+        <v>259</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','çay','Final','çay.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" t="s">
+        <v>251</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','karpuz','Final','karpuz.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>237</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','bebek','Blended','bebek.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" t="s">
+        <v>257</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('c','cüce','Blended','cüce.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" t="s">
+        <v>114</v>
+      </c>
+      <c r="D58" t="s">
+        <v>238</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','çiçek','Blended','çiçek.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','dede','Blended','dede.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" t="s">
+        <v>245</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fotograf','Blended','fotograf.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" t="s">
+        <v>114</v>
+      </c>
+      <c r="D61" t="s">
+        <v>240</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gaga','Blended','gaga.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" t="s">
+        <v>248</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','bakkal','Blended','bakkal.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" t="s">
+        <v>252</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lale','Blended','lale.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>114</v>
+      </c>
+      <c r="D64" t="s">
+        <v>241</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mum','Blended','mum.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" t="s">
+        <v>247</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','ananas','Blended','ananas.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D66" t="s">
+        <v>242</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','paspas','Blended','paspas.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" t="s">
+        <v>243</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E73" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"', 'TR');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','rüzgar','Blended','rüzgar.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C68" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" t="s">
+        <v>255</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','seksen','Blended','seksen.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69" t="s">
+        <v>114</v>
+      </c>
+      <c r="D69" t="s">
+        <v>260</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','şişman','Blended','şişman.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" t="s">
+        <v>256</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tablet','Blended','tablet.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" t="s">
+        <v>249</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','civciv','Blended','civciv.jpg', 'TR');</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" t="s">
+        <v>244</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yay','Blended','yay.png', 'TR');</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C73" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" t="s">
+        <v>261</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','gazoz','Blended','gazoz.jpg', 'TR');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14D73E8-9D7A-447F-B50C-ED6B4869D891}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worksheets Pdfviewer Added English Articulation test & Images
</commit_message>
<xml_diff>
--- a/Doc/articulation_test_eng.xlsx
+++ b/Doc/articulation_test_eng.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SpeechPathology\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5246E9-BA88-48B1-A587-CF551B7F4CA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611EE717-EC24-4ECC-9349-126CD404B85C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3" xr2:uid="{DDB625DF-4F01-4CCA-920B-D59ABAD0D606}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{DDB625DF-4F01-4CCA-920B-D59ABAD0D606}"/>
   </bookViews>
   <sheets>
     <sheet name="ENG_DATA" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ENG_SQL!$A$1:$E$81</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="260">
   <si>
     <t>Sounds</t>
   </si>
@@ -377,12 +377,6 @@
   </si>
   <si>
     <t>Blended</t>
-  </si>
-  <si>
-    <t>lemon.jpg</t>
-  </si>
-  <si>
-    <t>book.jpg</t>
   </si>
   <si>
     <t>LETTER</t>
@@ -1717,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ED3D1D-554F-4288-BEE9-9630FEF3B2C4}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,12 +1749,13 @@
       <c r="C2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" t="s">
-        <v>116</v>
+      <c r="D2" t="str">
+        <f>B2&amp;".jpg"</f>
+        <v>mole.jpg</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','mole','Initial','book.jpg');</v>
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mole','Initial','mole.jpg', 'EN');</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1773,12 +1768,13 @@
       <c r="C3" t="s">
         <v>111</v>
       </c>
-      <c r="D3" t="s">
-        <v>115</v>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="0">B3&amp;".jpg"</f>
+        <v>nut.jpg</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','nut','Initial','lemon.jpg');</v>
+        <f t="shared" ref="E3:E66" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','nut','Initial','nut.jpg', 'EN');</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1791,12 +1787,13 @@
       <c r="C4" t="s">
         <v>111</v>
       </c>
-      <c r="D4" t="s">
-        <v>115</v>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>hen.jpg</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('h','hen','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hen','Initial','hen.jpg', 'EN');</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1809,12 +1806,13 @@
       <c r="C5" t="s">
         <v>111</v>
       </c>
-      <c r="D5" t="s">
-        <v>116</v>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>pig.jpg</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','pig','Initial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pig','Initial','pig.jpg', 'EN');</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1827,12 +1825,13 @@
       <c r="C6" t="s">
         <v>111</v>
       </c>
-      <c r="D6" t="s">
-        <v>115</v>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>boot.jpg</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','boot','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','boot','Initial','boot.jpg', 'EN');</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1845,12 +1844,13 @@
       <c r="C7" t="s">
         <v>111</v>
       </c>
-      <c r="D7" t="s">
-        <v>116</v>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>train.jpg</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','train','Initial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','train','Initial','train.jpg', 'EN');</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1863,12 +1863,13 @@
       <c r="C8" t="s">
         <v>111</v>
       </c>
-      <c r="D8" t="s">
-        <v>115</v>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>cat.jpg</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','cat','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cat','Initial','cat.jpg', 'EN');</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1881,12 +1882,13 @@
       <c r="C9" t="s">
         <v>111</v>
       </c>
-      <c r="D9" t="s">
-        <v>115</v>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>wolf.jpg</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','wolf','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','wolf','Initial','wolf.jpg', 'EN');</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1899,12 +1901,13 @@
       <c r="C10" t="s">
         <v>111</v>
       </c>
-      <c r="D10" t="s">
-        <v>115</v>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>dog.jpg</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','dog','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','dog','Initial','dog.jpg', 'EN');</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1917,12 +1920,13 @@
       <c r="C11" t="s">
         <v>111</v>
       </c>
-      <c r="D11" t="s">
-        <v>115</v>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>gate.jpg</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','gate','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gate','Initial','gate.jpg', 'EN');</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1935,12 +1939,13 @@
       <c r="C12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
-        <v>116</v>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>finger.jpg</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','finger','Initial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','finger','Initial','finger.jpg', 'EN');</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1953,12 +1958,13 @@
       <c r="C13" t="s">
         <v>111</v>
       </c>
-      <c r="D13" t="s">
-        <v>115</v>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>log.jpg</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','log','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','log','Initial','log.jpg', 'EN');</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1971,12 +1977,13 @@
       <c r="C14" t="s">
         <v>111</v>
       </c>
-      <c r="D14" t="s">
-        <v>116</v>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>sun.jpg</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','sun','Initial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','sun','Initial','sun.jpg', 'EN');</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1989,12 +1996,13 @@
       <c r="C15" t="s">
         <v>111</v>
       </c>
-      <c r="D15" t="s">
-        <v>115</v>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>van.jpg</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('v','van','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','van','Initial','van.jpg', 'EN');</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2007,12 +2015,13 @@
       <c r="C16" t="s">
         <v>111</v>
       </c>
-      <c r="D16" t="s">
-        <v>115</v>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>yak.jpg</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','yak','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yak','Initial','yak.jpg', 'EN');</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2025,12 +2034,13 @@
       <c r="C17" t="s">
         <v>111</v>
       </c>
-      <c r="D17" t="s">
-        <v>115</v>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>chips.jpg</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','chips','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','chips','Initial','chips.jpg', 'EN');</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2043,12 +2053,13 @@
       <c r="C18" t="s">
         <v>111</v>
       </c>
-      <c r="D18" t="s">
-        <v>115</v>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>rat.jpg</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','rat','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','rat','Initial','rat.jpg', 'EN');</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2061,12 +2072,13 @@
       <c r="C19" t="s">
         <v>111</v>
       </c>
-      <c r="D19" t="s">
-        <v>115</v>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>jam.jpg</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','jam','Initial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','jam','Initial','jam.jpg', 'EN');</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2079,12 +2091,13 @@
       <c r="C20" t="s">
         <v>111</v>
       </c>
-      <c r="D20" t="s">
-        <v>116</v>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>shower.jpg</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('sh','shower','Initial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','shower','Initial','shower.jpg', 'EN');</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2097,12 +2110,13 @@
       <c r="C21" t="s">
         <v>111</v>
       </c>
-      <c r="D21" t="s">
-        <v>116</v>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>thistle.jpg</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('th','thistle','Initial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','thistle','Initial','thistle.jpg', 'EN');</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2115,12 +2129,13 @@
       <c r="C22" t="s">
         <v>112</v>
       </c>
-      <c r="D22" t="s">
-        <v>115</v>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>lemon.jpg</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','lemon','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','lemon','Medial','lemon.jpg', 'EN');</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2133,12 +2148,13 @@
       <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="D23" t="s">
-        <v>116</v>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>dinner.jpg</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','dinner','Medial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','dinner','Medial','dinner.jpg', 'EN');</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2151,12 +2167,13 @@
       <c r="C24" t="s">
         <v>112</v>
       </c>
-      <c r="D24" t="s">
-        <v>115</v>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>foghorn.jpg</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('h','foghorn','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','foghorn','Medial','foghorn.jpg', 'EN');</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2169,12 +2186,13 @@
       <c r="C25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" t="s">
-        <v>115</v>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>slipper.jpg</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','slipper','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','slipper','Medial','slipper.jpg', 'EN');</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2187,12 +2205,13 @@
       <c r="C26" t="s">
         <v>112</v>
       </c>
-      <c r="D26" t="s">
-        <v>115</v>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>robot.jpg</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','robot','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','robot','Medial','robot.jpg', 'EN');</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2205,12 +2224,13 @@
       <c r="C27" t="s">
         <v>112</v>
       </c>
-      <c r="D27" t="s">
-        <v>115</v>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>water.jpg</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','water','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','water','Medial','water.jpg', 'EN');</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2223,12 +2243,13 @@
       <c r="C28" t="s">
         <v>112</v>
       </c>
-      <c r="D28" t="s">
-        <v>115</v>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>rocket.jpg</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','rocket','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','rocket','Medial','rocket.jpg', 'EN');</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2241,12 +2262,13 @@
       <c r="C29" t="s">
         <v>112</v>
       </c>
-      <c r="D29" t="s">
-        <v>115</v>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>tower.jpg</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','tower','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','tower','Medial','tower.jpg', 'EN');</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2259,12 +2281,13 @@
       <c r="C30" t="s">
         <v>112</v>
       </c>
-      <c r="D30" t="s">
-        <v>115</v>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>puddle.jpg</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','puddle','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','puddle','Medial','puddle.jpg', 'EN');</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2277,12 +2300,13 @@
       <c r="C31" t="s">
         <v>112</v>
       </c>
-      <c r="D31" t="s">
-        <v>115</v>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>tiger.jpg</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','tiger','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','tiger','Medial','tiger.jpg', 'EN');</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -2295,12 +2319,13 @@
       <c r="C32" t="s">
         <v>112</v>
       </c>
-      <c r="D32" t="s">
-        <v>116</v>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>wafer.jpg</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','wafer','Medial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','wafer','Medial','wafer.jpg', 'EN');</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -2313,12 +2338,13 @@
       <c r="C33" t="s">
         <v>112</v>
       </c>
-      <c r="D33" t="s">
-        <v>115</v>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>finger.jpg</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ng','finger','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','finger','Medial','finger.jpg', 'EN');</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -2331,12 +2357,13 @@
       <c r="C34" t="s">
         <v>112</v>
       </c>
-      <c r="D34" t="s">
-        <v>116</v>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>tulip.jpg</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','tulip','Medial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','tulip','Medial','tulip.jpg', 'EN');</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2349,12 +2376,13 @@
       <c r="C35" t="s">
         <v>112</v>
       </c>
-      <c r="D35" t="s">
-        <v>115</v>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>buses.jpg</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','buses','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','buses','Medial','buses.jpg', 'EN');</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -2367,12 +2395,13 @@
       <c r="C36" t="s">
         <v>112</v>
       </c>
-      <c r="D36" t="s">
-        <v>115</v>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>waving.jpg</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('v','waving','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','waving','Medial','waving.jpg', 'EN');</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -2385,12 +2414,13 @@
       <c r="C37" t="s">
         <v>112</v>
       </c>
-      <c r="D37" t="s">
-        <v>115</v>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>crayon.jpg</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','crayon','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','crayon','Medial','crayon.jpg', 'EN');</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2403,12 +2433,13 @@
       <c r="C38" t="s">
         <v>112</v>
       </c>
-      <c r="D38" t="s">
-        <v>115</v>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>archer.jpg</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','archer','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','archer','Medial','archer.jpg', 'EN');</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -2421,12 +2452,13 @@
       <c r="C39" t="s">
         <v>112</v>
       </c>
-      <c r="D39" t="s">
-        <v>116</v>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>barrel.jpg</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','barrel','Medial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','barrel','Medial','barrel.jpg', 'EN');</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -2439,12 +2471,13 @@
       <c r="C40" t="s">
         <v>112</v>
       </c>
-      <c r="D40" t="s">
-        <v>115</v>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>badger.jpg</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','badger','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','badger','Medial','badger.jpg', 'EN');</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -2457,12 +2490,13 @@
       <c r="C41" t="s">
         <v>112</v>
       </c>
-      <c r="D41" t="s">
-        <v>115</v>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>bishop.jpg</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('sh','bishop','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','bishop','Medial','bishop.jpg', 'EN');</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -2475,12 +2509,13 @@
       <c r="C42" t="s">
         <v>112</v>
       </c>
-      <c r="D42" t="s">
-        <v>116</v>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>father.jpg</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('th','father','Medial','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','father','Medial','father.jpg', 'EN');</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -2493,12 +2528,13 @@
       <c r="C43" t="s">
         <v>112</v>
       </c>
-      <c r="D43" t="s">
-        <v>115</v>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>measure.jpg</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('zh','measure','Medial','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('zh','measure','Medial','measure.jpg', 'EN');</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2511,12 +2547,13 @@
       <c r="C44" t="s">
         <v>113</v>
       </c>
-      <c r="D44" t="s">
-        <v>115</v>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>thumb.jpg</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','thumb','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','thumb','Final','thumb.jpg', 'EN');</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2529,12 +2566,13 @@
       <c r="C45" t="s">
         <v>113</v>
       </c>
-      <c r="D45" t="s">
-        <v>115</v>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>pin.jpg</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','pin','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','pin','Final','pin.jpg', 'EN');</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2547,12 +2585,13 @@
       <c r="C46" t="s">
         <v>113</v>
       </c>
-      <c r="D46" t="s">
-        <v>115</v>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>map.jpg</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','map','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','map','Final','map.jpg', 'EN');</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -2565,12 +2604,13 @@
       <c r="C47" t="s">
         <v>113</v>
       </c>
-      <c r="D47" t="s">
-        <v>115</v>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>cub.jpg</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','cub','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','cub','Final','cub.jpg', 'EN');</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -2583,12 +2623,13 @@
       <c r="C48" t="s">
         <v>113</v>
       </c>
-      <c r="D48" t="s">
-        <v>115</v>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>hat.jpg</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','hat','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','hat','Final','hat.jpg', 'EN');</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2601,12 +2642,13 @@
       <c r="C49" t="s">
         <v>113</v>
       </c>
-      <c r="D49" t="s">
-        <v>116</v>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>sock.jpg</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','sock','Final','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','sock','Final','sock.jpg', 'EN');</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -2619,12 +2661,13 @@
       <c r="C50" t="s">
         <v>113</v>
       </c>
-      <c r="D50" t="s">
-        <v>115</v>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>cow.jpg</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','cow','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','cow','Final','cow.jpg', 'EN');</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -2637,12 +2680,13 @@
       <c r="C51" t="s">
         <v>113</v>
       </c>
-      <c r="D51" t="s">
-        <v>115</v>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>head.jpg</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','head','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','head','Final','head.jpg', 'EN');</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2655,12 +2699,13 @@
       <c r="C52" t="s">
         <v>113</v>
       </c>
-      <c r="D52" t="s">
-        <v>115</v>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>bag.jpg</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','bag','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','bag','Final','bag.jpg', 'EN');</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2673,12 +2718,13 @@
       <c r="C53" t="s">
         <v>113</v>
       </c>
-      <c r="D53" t="s">
-        <v>115</v>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>laugh.jpg</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','laugh','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','laugh','Final','laugh.jpg', 'EN');</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2691,12 +2737,13 @@
       <c r="C54" t="s">
         <v>113</v>
       </c>
-      <c r="D54" t="s">
-        <v>115</v>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>wing.jpg</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ng','wing','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','wing','Final','wing.jpg', 'EN');</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2709,12 +2756,13 @@
       <c r="C55" t="s">
         <v>113</v>
       </c>
-      <c r="D55" t="s">
-        <v>116</v>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>hill.jpg</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','hill','Final','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','hill','Final','hill.jpg', 'EN');</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2727,12 +2775,13 @@
       <c r="C56" t="s">
         <v>113</v>
       </c>
-      <c r="D56" t="s">
-        <v>115</v>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>moose.jpg</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','moose','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','moose','Final','moose.jpg', 'EN');</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2745,12 +2794,13 @@
       <c r="C57" t="s">
         <v>113</v>
       </c>
-      <c r="D57" t="s">
-        <v>115</v>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>sieve.jpg</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('v','sieve','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','sieve','Final','sieve.jpg', 'EN');</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2763,12 +2813,13 @@
       <c r="C58" t="s">
         <v>113</v>
       </c>
-      <c r="D58" t="s">
-        <v>116</v>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>toy.jpg</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','toy','Final','book.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','toy','Final','toy.jpg', 'EN');</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2781,12 +2832,13 @@
       <c r="C59" t="s">
         <v>113</v>
       </c>
-      <c r="D59" t="s">
-        <v>115</v>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>witch.jpg</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','witch','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','witch','Final','witch.jpg', 'EN');</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2799,12 +2851,13 @@
       <c r="C60" t="s">
         <v>113</v>
       </c>
-      <c r="D60" t="s">
-        <v>115</v>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>car.jpg</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','car','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','car','Final','car.jpg', 'EN');</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2817,12 +2870,13 @@
       <c r="C61" t="s">
         <v>113</v>
       </c>
-      <c r="D61" t="s">
-        <v>115</v>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>midge.jpg</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','midge','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','midge','Final','midge.jpg', 'EN');</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2835,12 +2889,13 @@
       <c r="C62" t="s">
         <v>113</v>
       </c>
-      <c r="D62" t="s">
-        <v>115</v>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>fish.jpg</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('sh','fish','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','fish','Final','fish.jpg', 'EN');</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2853,12 +2908,13 @@
       <c r="C63" t="s">
         <v>113</v>
       </c>
-      <c r="D63" t="s">
-        <v>115</v>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>path.jpg</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('th','path','Final','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','path','Final','path.jpg', 'EN');</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2871,12 +2927,13 @@
       <c r="C64" t="s">
         <v>114</v>
       </c>
-      <c r="D64" t="s">
-        <v>115</v>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>mummy.jpg</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('m','mummy','Blended','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mummy','Blended','mummy.jpg', 'EN');</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2889,12 +2946,13 @@
       <c r="C65" t="s">
         <v>114</v>
       </c>
-      <c r="D65" t="s">
-        <v>115</v>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>cannon.jpg</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('n','cannon','Blended','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','cannon','Blended','cannon.jpg', 'EN');</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2907,12 +2965,13 @@
       <c r="C66" t="s">
         <v>114</v>
       </c>
-      <c r="D66" t="s">
-        <v>115</v>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>hardhat.jpg</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('h','hardhat','Blended','lemon.jpg');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hardhat','Blended','hardhat.jpg', 'EN');</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -2925,12 +2984,13 @@
       <c r="C67" t="s">
         <v>114</v>
       </c>
-      <c r="D67" t="s">
-        <v>116</v>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D81" si="2">B67&amp;".jpg"</f>
+        <v>pepper.jpg</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E81" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('p','pepper','Blended','book.jpg');</v>
+        <f t="shared" ref="E67:E81" si="3">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pepper','Blended','pepper.jpg', 'EN');</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -2943,12 +3003,13 @@
       <c r="C68" t="s">
         <v>114</v>
       </c>
-      <c r="D68" t="s">
-        <v>115</v>
+      <c r="D68" t="str">
+        <f t="shared" si="2"/>
+        <v>baby.jpg</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('b','baby','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','baby','Blended','baby.jpg', 'EN');</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2961,12 +3022,13 @@
       <c r="C69" t="s">
         <v>114</v>
       </c>
-      <c r="D69" t="s">
-        <v>115</v>
+      <c r="D69" t="str">
+        <f t="shared" si="2"/>
+        <v>tent.jpg</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('t','tent','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tent','Blended','tent.jpg', 'EN');</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -2979,12 +3041,13 @@
       <c r="C70" t="s">
         <v>114</v>
       </c>
-      <c r="D70" t="s">
-        <v>116</v>
+      <c r="D70" t="str">
+        <f t="shared" si="2"/>
+        <v>cockerel.jpg</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('k','cockerel','Blended','book.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cockerel','Blended','cockerel.jpg', 'EN');</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2997,12 +3060,13 @@
       <c r="C71" t="s">
         <v>114</v>
       </c>
-      <c r="D71" t="s">
-        <v>115</v>
+      <c r="D71" t="str">
+        <f t="shared" si="2"/>
+        <v>window.jpg</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('w','window','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','window','Blended','window.jpg', 'EN');</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -3015,12 +3079,13 @@
       <c r="C72" t="s">
         <v>114</v>
       </c>
-      <c r="D72" t="s">
-        <v>115</v>
+      <c r="D72" t="str">
+        <f t="shared" si="2"/>
+        <v>daddy.jpg</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('d','daddy','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','daddy','Blended','daddy.jpg', 'EN');</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -3033,12 +3098,13 @@
       <c r="C73" t="s">
         <v>114</v>
       </c>
-      <c r="D73" t="s">
-        <v>115</v>
+      <c r="D73" t="str">
+        <f t="shared" si="2"/>
+        <v>goggles.jpg</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('g','goggles','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','goggles','Blended','goggles.jpg', 'EN');</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,12 +3117,13 @@
       <c r="C74" t="s">
         <v>114</v>
       </c>
-      <c r="D74" t="s">
-        <v>115</v>
+      <c r="D74" t="str">
+        <f t="shared" si="2"/>
+        <v>fifteen.jpg</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('f','fifteen','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fifteen','Blended','fifteen.jpg', 'EN');</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -3069,12 +3136,13 @@
       <c r="C75" t="s">
         <v>114</v>
       </c>
-      <c r="D75" t="s">
-        <v>116</v>
+      <c r="D75" t="str">
+        <f t="shared" si="2"/>
+        <v>swinging.jpg</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ng','swinging','Blended','book.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','swinging','Blended','swinging.jpg', 'EN');</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -3087,12 +3155,13 @@
       <c r="C76" t="s">
         <v>114</v>
       </c>
-      <c r="D76" t="s">
-        <v>115</v>
+      <c r="D76" t="str">
+        <f t="shared" si="2"/>
+        <v>lollipop.jpg</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('l','lollipop','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lollipop','Blended','lollipop.jpg', 'EN');</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -3105,12 +3174,13 @@
       <c r="C77" t="s">
         <v>114</v>
       </c>
-      <c r="D77" t="s">
-        <v>115</v>
+      <c r="D77" t="str">
+        <f t="shared" si="2"/>
+        <v>buses.jpg</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('s','buses','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','buses','Blended','buses.jpg', 'EN');</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -3123,12 +3193,13 @@
       <c r="C78" t="s">
         <v>114</v>
       </c>
-      <c r="D78" t="s">
-        <v>116</v>
+      <c r="D78" t="str">
+        <f t="shared" si="2"/>
+        <v>yoyo.jpg</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('y','yoyo','Blended','book.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yoyo','Blended','yoyo.jpg', 'EN');</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -3141,12 +3212,13 @@
       <c r="C79" t="s">
         <v>114</v>
       </c>
-      <c r="D79" t="s">
-        <v>115</v>
+      <c r="D79" t="str">
+        <f t="shared" si="2"/>
+        <v>church.jpg</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('ch','church','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','church','Blended','church.jpg', 'EN');</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -3159,12 +3231,13 @@
       <c r="C80" t="s">
         <v>114</v>
       </c>
-      <c r="D80" t="s">
-        <v>115</v>
+      <c r="D80" t="str">
+        <f t="shared" si="2"/>
+        <v>robber.jpg</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('r','robber','Blended','lemon.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','robber','Blended','robber.jpg', 'EN');</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -3177,12 +3250,13 @@
       <c r="C81" t="s">
         <v>114</v>
       </c>
-      <c r="D81" t="s">
-        <v>116</v>
+      <c r="D81" t="str">
+        <f t="shared" si="2"/>
+        <v>george.jpg</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image])  VALUES ('j','george','Blended','book.jpg');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','george','Blended','george.jpg', 'EN');</v>
       </c>
     </row>
   </sheetData>
@@ -3205,7 +3279,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -3225,46 +3299,46 @@
         <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3272,14 +3346,14 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -3287,16 +3361,16 @@
         <v>55</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3304,16 +3378,16 @@
         <v>50</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3321,13 +3395,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -3336,16 +3410,16 @@
         <v>35</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -3353,16 +3427,16 @@
         <v>63</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -3370,16 +3444,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -3387,16 +3461,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -3404,16 +3478,16 @@
         <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -3421,16 +3495,16 @@
         <v>86</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -3438,33 +3512,33 @@
         <v>68</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3472,16 +3546,16 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -3489,16 +3563,16 @@
         <v>72</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3506,33 +3580,33 @@
         <v>76</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3544,8 +3618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7C40D4-1A8C-49B8-AC4C-BD9FDA66D6CE}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3576,13 +3650,13 @@
         <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"', 'TR');")</f>
@@ -3591,16 +3665,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"', 'TR');")</f>
@@ -3609,16 +3683,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -3630,13 +3704,13 @@
         <v>45</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -3648,13 +3722,13 @@
         <v>55</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
         <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -3666,13 +3740,13 @@
         <v>50</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -3684,13 +3758,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
         <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -3702,13 +3776,13 @@
         <v>35</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3720,13 +3794,13 @@
         <v>63</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
         <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -3738,13 +3812,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
         <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -3756,13 +3830,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
         <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -3774,13 +3848,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
         <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -3792,13 +3866,13 @@
         <v>86</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -3810,13 +3884,13 @@
         <v>68</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
         <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -3825,16 +3899,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
         <v>111</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -3846,13 +3920,13 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C17" t="s">
         <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -3864,13 +3938,13 @@
         <v>72</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
         <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -3882,13 +3956,13 @@
         <v>76</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C19" t="s">
         <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -3897,16 +3971,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C20" t="s">
         <v>111</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -3918,13 +3992,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
         <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -3933,16 +4007,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="C22" t="s">
         <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -3951,16 +4025,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="C23" t="s">
         <v>112</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -3972,13 +4046,13 @@
         <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
         <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -3990,13 +4064,13 @@
         <v>55</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
         <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -4008,13 +4082,13 @@
         <v>50</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s">
         <v>112</v>
       </c>
       <c r="D26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -4026,13 +4100,13 @@
         <v>15</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
         <v>112</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
@@ -4044,13 +4118,13 @@
         <v>35</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
         <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
@@ -4062,13 +4136,13 @@
         <v>63</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
         <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
@@ -4080,13 +4154,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C30" t="s">
         <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
@@ -4098,13 +4172,13 @@
         <v>10</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C31" t="s">
         <v>112</v>
       </c>
       <c r="D31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
@@ -4116,13 +4190,13 @@
         <v>20</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
         <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
@@ -4134,13 +4208,13 @@
         <v>86</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
         <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
@@ -4152,13 +4226,13 @@
         <v>68</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
         <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
@@ -4167,16 +4241,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="C35" t="s">
         <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -4188,13 +4262,13 @@
         <v>30</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C36" t="s">
         <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
@@ -4206,13 +4280,13 @@
         <v>72</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C37" t="s">
         <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
@@ -4224,13 +4298,13 @@
         <v>76</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
         <v>112</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
@@ -4239,16 +4313,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="C39" t="s">
         <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
@@ -4257,16 +4331,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C40" t="s">
         <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
@@ -4278,13 +4352,13 @@
         <v>55</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
         <v>113</v>
       </c>
       <c r="D41" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
@@ -4296,13 +4370,13 @@
         <v>50</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
         <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
@@ -4314,13 +4388,13 @@
         <v>15</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s">
         <v>113</v>
       </c>
       <c r="D43" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
@@ -4332,13 +4406,13 @@
         <v>35</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C44" t="s">
         <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
@@ -4350,13 +4424,13 @@
         <v>63</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
         <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
@@ -4368,13 +4442,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
         <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
@@ -4386,13 +4460,13 @@
         <v>10</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
         <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -4404,13 +4478,13 @@
         <v>20</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
         <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -4422,13 +4496,13 @@
         <v>86</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
         <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -4440,13 +4514,13 @@
         <v>68</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C50" t="s">
         <v>113</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -4455,16 +4529,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C51" t="s">
         <v>113</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -4476,13 +4550,13 @@
         <v>30</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
         <v>113</v>
       </c>
       <c r="D52" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
@@ -4494,13 +4568,13 @@
         <v>72</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C53" t="s">
         <v>113</v>
       </c>
       <c r="D53" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
@@ -4512,13 +4586,13 @@
         <v>76</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C54" t="s">
         <v>113</v>
       </c>
       <c r="D54" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
@@ -4527,16 +4601,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C55" t="s">
         <v>113</v>
       </c>
       <c r="D55" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
@@ -4548,13 +4622,13 @@
         <v>25</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
         <v>114</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
@@ -4563,16 +4637,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
         <v>114</v>
       </c>
       <c r="D57" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
@@ -4581,16 +4655,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
         <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
@@ -4602,13 +4676,13 @@
         <v>45</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
@@ -4620,13 +4694,13 @@
         <v>55</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
         <v>114</v>
       </c>
       <c r="D60" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
@@ -4638,13 +4712,13 @@
         <v>50</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C61" t="s">
         <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
@@ -4656,13 +4730,13 @@
         <v>35</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C62" t="s">
         <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
@@ -4674,13 +4748,13 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C63" t="s">
         <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
@@ -4692,13 +4766,13 @@
         <v>5</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
         <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
@@ -4710,13 +4784,13 @@
         <v>10</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C65" t="s">
         <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
@@ -4728,13 +4802,13 @@
         <v>20</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C66" t="s">
         <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
@@ -4746,13 +4820,13 @@
         <v>86</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
         <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" ref="E67:E73" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"', 'TR');")</f>
@@ -4764,13 +4838,13 @@
         <v>68</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C68" t="s">
         <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="1"/>
@@ -4779,16 +4853,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C69" t="s">
         <v>114</v>
       </c>
       <c r="D69" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="1"/>
@@ -4800,13 +4874,13 @@
         <v>30</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C70" t="s">
         <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
@@ -4818,13 +4892,13 @@
         <v>72</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C71" t="s">
         <v>114</v>
       </c>
       <c r="D71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
@@ -4836,13 +4910,13 @@
         <v>76</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C72" t="s">
         <v>114</v>
       </c>
       <c r="D72" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
@@ -4851,16 +4925,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C73" t="s">
         <v>114</v>
       </c>
       <c r="D73" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>

</xml_diff>